<commit_message>
oops new truth tbale
</commit_message>
<xml_diff>
--- a/Lab7/Control Unit Truth Table.xlsx
+++ b/Lab7/Control Unit Truth Table.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITS\140Labs\CMPE140Labs\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5927374B-1DD6-47E1-B790-E7358EEC5FD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0380FD0-6A93-490B-A484-9F4C8F043236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29790" yWindow="6375" windowWidth="15225" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="4125" windowWidth="15225" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
   <si>
     <t>alu_ctrl</t>
   </si>
@@ -143,9 +142,6 @@
     <t>wbmux1_sel</t>
   </si>
   <si>
-    <t>wbmux2_sel</t>
-  </si>
-  <si>
     <t>wbmux3_sel</t>
   </si>
   <si>
@@ -158,7 +154,7 @@
     <t>SLR</t>
   </si>
   <si>
-    <t>jump_return</t>
+    <t>left_or_right</t>
   </si>
 </sst>
 </file>
@@ -424,10 +420,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -435,7 +431,7 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -447,25 +443,19 @@
         <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -478,7 +468,7 @@
       <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2">
         <v>0</v>
       </c>
       <c r="F2">
@@ -490,14 +480,8 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -510,7 +494,7 @@
       <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
@@ -522,166 +506,155 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -689,16 +662,10 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -707,30 +674,24 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+      <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
         <v>1</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -739,30 +700,24 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2">
+        <v>9</v>
+      </c>
+      <c r="E11">
         <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
@@ -773,26 +728,20 @@
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
@@ -805,90 +754,26 @@
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13">
         <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
@@ -940,7 +825,9 @@
       <c r="I24" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J24" s="1"/>
+      <c r="J24" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
@@ -970,7 +857,9 @@
       <c r="I25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="3"/>
+      <c r="J25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
@@ -1000,7 +889,9 @@
       <c r="I26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J26" s="3"/>
+      <c r="J26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
@@ -1030,11 +921,13 @@
       <c r="I27" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J27" s="3"/>
+      <c r="J27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
@@ -1060,7 +953,9 @@
       <c r="I28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="3"/>
+      <c r="J28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
@@ -1090,7 +985,9 @@
       <c r="I29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="3"/>
+      <c r="J29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
@@ -1120,31 +1017,41 @@
       <c r="I30" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J30" s="3"/>
+      <c r="J30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J33" s="3"/>
-    </row>
-    <row r="34" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="10:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J35" s="3"/>
+      <c r="A31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding working copy of lab 7
</commit_message>
<xml_diff>
--- a/Lab7/Control Unit Truth Table.xlsx
+++ b/Lab7/Control Unit Truth Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITS\140Labs\CMPE140Labs\Lab7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\School\CMPE 140\CMPE140Labs\Lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0380FD0-6A93-490B-A484-9F4C8F043236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5539F2-6D9D-44EB-A7FB-920B8202666B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4125" windowWidth="15225" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24285" yWindow="1710" windowWidth="23760" windowHeight="17145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="45">
   <si>
     <t>alu_ctrl</t>
   </si>
@@ -420,10 +420,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -561,10 +561,10 @@
     </row>
     <row r="6" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>9</v>
@@ -587,13 +587,13 @@
     </row>
     <row r="7" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
@@ -612,23 +612,23 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
+      <c r="A8" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="9" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
@@ -648,10 +648,10 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="10" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -674,13 +674,13 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="11" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -709,15 +709,15 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
@@ -738,49 +738,33 @@
         <v>1</v>
       </c>
       <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
+    </row>
+    <row r="13" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:8" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
     <row r="22" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -791,47 +775,69 @@
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>37</v>
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
@@ -840,13 +846,13 @@
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>4</v>
@@ -855,54 +861,54 @@
         <v>4</v>
       </c>
       <c r="I25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="D27" s="3" t="s">
         <v>4</v>
       </c>
@@ -919,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J27">
         <v>0</v>
@@ -927,13 +933,13 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
@@ -942,10 +948,10 @@
         <v>4</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>4</v>
@@ -959,7 +965,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>4</v>
@@ -971,16 +977,16 @@
         <v>4</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>4</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>9</v>
@@ -991,13 +997,13 @@
     </row>
     <row r="30" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
@@ -1006,50 +1012,18 @@
         <v>16</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="J30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31">
         <v>1</v>
       </c>
     </row>

</xml_diff>